<commit_message>
add more to summarya
add more to summarya
</commit_message>
<xml_diff>
--- a/Case Study 7/Data Summary QTW final.xlsx
+++ b/Case Study 7/Data Summary QTW final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjsch\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jjschued\Documents\GitHub\7333QTW\Case Study 7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEE3B567-0538-4270-B634-82F35B617BBA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9A0E9AD-304F-4C5D-AAF9-96B1A0DFE929}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{AB6B9DB5-2A84-4B58-8472-1E1AF0154493}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{AB6B9DB5-2A84-4B58-8472-1E1AF0154493}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,6 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,41 +42,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="102">
-  <si>
-    <t>asia</t>
-  </si>
-  <si>
-    <t>euorpe</t>
-  </si>
-  <si>
-    <t>america</t>
-  </si>
-  <si>
-    <t>NaN</t>
-  </si>
-  <si>
-    <t>wednesday</t>
-  </si>
-  <si>
-    <t>thurday</t>
-  </si>
-  <si>
-    <t>tuesday</t>
-  </si>
-  <si>
-    <t>friday</t>
-  </si>
-  <si>
-    <t>monday</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="104">
   <si>
     <t>Unique</t>
   </si>
   <si>
-    <t>July</t>
-  </si>
-  <si>
     <t>Jun</t>
   </si>
   <si>
@@ -87,9 +56,6 @@
     <t>May</t>
   </si>
   <si>
-    <t>sept.</t>
-  </si>
-  <si>
     <t>Mar</t>
   </si>
   <si>
@@ -99,9 +65,6 @@
     <t>Feb</t>
   </si>
   <si>
-    <t>Dev</t>
-  </si>
-  <si>
     <t>Jan</t>
   </si>
   <si>
@@ -349,6 +312,48 @@
   </si>
   <si>
     <t>Uniques</t>
+  </si>
+  <si>
+    <t>Sep</t>
+  </si>
+  <si>
+    <t>Jul</t>
+  </si>
+  <si>
+    <t>Dec</t>
+  </si>
+  <si>
+    <t>Asia</t>
+  </si>
+  <si>
+    <t>America</t>
+  </si>
+  <si>
+    <t>Float</t>
+  </si>
+  <si>
+    <t>Interger</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>Thursday</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>Europe</t>
   </si>
 </sst>
 </file>
@@ -1208,61 +1213,62 @@
   <dimension ref="B2:L33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.53125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="11" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="G2" s="4"/>
       <c r="H2" s="11" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I2" s="11" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="11" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
-        <v>0</v>
+        <v>93</v>
       </c>
       <c r="C3" s="10">
         <v>138965</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="6" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="F3" s="10">
         <v>45569</v>
       </c>
       <c r="G3" s="4"/>
       <c r="H3" s="6" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="I3" s="10">
         <v>101535</v>
@@ -1275,23 +1281,23 @@
         <v>40767</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
-        <v>1</v>
+        <v>103</v>
       </c>
       <c r="C4" s="10">
         <v>16538</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="6" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F4" s="10">
         <v>41329</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="6" t="s">
-        <v>5</v>
+        <v>99</v>
       </c>
       <c r="I4" s="10">
         <v>29429</v>
@@ -1304,23 +1310,23 @@
         <v>34094</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" s="6" t="s">
-        <v>2</v>
+        <v>94</v>
       </c>
       <c r="C5" s="10">
         <v>4469</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="6" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F5" s="10">
         <v>29406</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="6" t="s">
-        <v>6</v>
+        <v>100</v>
       </c>
       <c r="I5" s="10">
         <v>27954</v>
@@ -1333,23 +1339,19 @@
         <v>33923</v>
       </c>
     </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
-      <c r="B6" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="10">
-        <v>28</v>
-      </c>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="F6" s="10">
         <v>21939</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="6" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="I6" s="10">
         <v>564</v>
@@ -1362,19 +1364,19 @@
         <v>30492</v>
       </c>
     </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
       <c r="E7" s="6" t="s">
-        <v>14</v>
+        <v>90</v>
       </c>
       <c r="F7" s="10">
         <v>10819</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="6" t="s">
-        <v>8</v>
+        <v>102</v>
       </c>
       <c r="I7" s="10">
         <v>488</v>
@@ -1387,23 +1389,19 @@
         <v>9924</v>
       </c>
     </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" s="5"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
       <c r="E8" s="7" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="F8" s="10">
         <v>6761</v>
       </c>
       <c r="G8" s="4"/>
-      <c r="H8" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="10">
-        <v>30</v>
-      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="9">
         <v>2.0000000000000001E-4</v>
@@ -1412,12 +1410,12 @@
         <v>7987</v>
       </c>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="F9" s="10">
         <v>2407</v>
@@ -1433,12 +1431,12 @@
         <v>1727</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
       <c r="E10" s="6" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="F10" s="10">
         <v>1231</v>
@@ -1454,12 +1452,12 @@
         <v>855</v>
       </c>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="6" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="F11" s="10">
         <v>337</v>
@@ -1475,12 +1473,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
       <c r="E12" s="6" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F12" s="10">
         <v>140</v>
@@ -1496,111 +1494,99 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
       <c r="E13" s="6" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="F13" s="10">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
-      <c r="K13" s="6" t="s">
-        <v>3</v>
+      <c r="K13" s="9">
+        <v>-5.0000000000000001E-4</v>
       </c>
       <c r="L13" s="10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="6" t="s">
-        <v>18</v>
+      <c r="E14" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="F14" s="10">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="9">
-        <v>-5.0000000000000001E-4</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="L14" s="10">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="10">
-        <v>8</v>
-      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
-      <c r="K15" s="9">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="L15" s="10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="11" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="6" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="C19" s="10">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="6" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="C20" s="10">
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="6" t="s">
-        <v>70</v>
+        <v>97</v>
       </c>
       <c r="C21" s="10">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B32" s="2"/>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="1"/>
     </row>
   </sheetData>
@@ -1628,55 +1614,55 @@
       </pivotSelection>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" s="13" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.45">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C4" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" s="14" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="C5" s="15">
         <v>45</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" s="14" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C6" s="15">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" s="14" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C7" s="15">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B8" s="14" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C8" s="15">
         <v>52</v>
@@ -1695,941 +1681,941 @@
       <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C1">
         <v>60000</v>
       </c>
       <c r="D1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="2" t="s">
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
         <v>30</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E4" t="s">
         <v>31</v>
       </c>
-      <c r="C2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" t="s">
-        <v>42</v>
-      </c>
-      <c r="E4" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C5">
         <v>159974</v>
       </c>
       <c r="D5" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C6">
         <v>159975</v>
       </c>
       <c r="D6" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="C7">
         <v>159962</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="C8">
         <v>159963</v>
       </c>
       <c r="D8" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E8" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="C9">
         <v>159974</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="C10">
         <v>159963</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C11">
         <v>159974</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="C12">
         <v>159973</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E12" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>159979</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>159970</v>
       </c>
       <c r="D14" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="C15">
         <v>159957</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E15" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>11</v>
       </c>
       <c r="B16" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C16">
         <v>159970</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="C17">
         <v>159964</v>
       </c>
       <c r="D17" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E17" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="C18">
         <v>159969</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>14</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="C19">
         <v>159966</v>
       </c>
       <c r="D19" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>15</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C20">
         <v>159965</v>
       </c>
       <c r="D20" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E20" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>16</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="C21">
         <v>159974</v>
       </c>
       <c r="D21" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>17</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="C22">
         <v>159973</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="C23">
         <v>159960</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>19</v>
       </c>
       <c r="B24" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="C24">
         <v>159965</v>
       </c>
       <c r="D24" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="C25">
         <v>159962</v>
       </c>
       <c r="D25" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="C26">
         <v>159971</v>
       </c>
       <c r="D26" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="C27">
         <v>159973</v>
       </c>
       <c r="D27" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E27" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="C28">
         <v>159953</v>
       </c>
       <c r="D28" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E28" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <v>159972</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E29" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="C30">
         <v>159978</v>
       </c>
       <c r="D30" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E30" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>26</v>
       </c>
       <c r="B31" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="C31">
         <v>159964</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E31" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C32">
         <v>159970</v>
       </c>
       <c r="D32" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E32" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>28</v>
       </c>
       <c r="B33" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="C33">
         <v>159965</v>
       </c>
       <c r="D33" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E33" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <v>159970</v>
       </c>
       <c r="D34" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>30</v>
       </c>
       <c r="B35" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="C35">
         <v>159970</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>31</v>
       </c>
       <c r="B36" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C36">
         <v>159961</v>
       </c>
       <c r="D36" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E36" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>32</v>
       </c>
       <c r="B37" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="C37">
         <v>159969</v>
       </c>
       <c r="D37" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E37" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>33</v>
       </c>
       <c r="B38" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="C38">
         <v>159959</v>
       </c>
       <c r="D38" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E38" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>34</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="C39">
         <v>159959</v>
       </c>
       <c r="D39" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E39" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>35</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="C40">
         <v>159970</v>
       </c>
       <c r="D40" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E40" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>36</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="C41">
         <v>159973</v>
       </c>
       <c r="D41" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E41" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>37</v>
       </c>
       <c r="B42" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="C42">
         <v>159977</v>
       </c>
       <c r="D42" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E42" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>38</v>
       </c>
       <c r="B43" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C43">
         <v>159969</v>
       </c>
       <c r="D43" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E43" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>39</v>
       </c>
       <c r="B44" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="C44">
         <v>159977</v>
       </c>
       <c r="D44" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E44" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>40</v>
       </c>
       <c r="B45" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C45">
         <v>159964</v>
       </c>
       <c r="D45" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E45" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C46">
         <v>159960</v>
       </c>
       <c r="D46" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E46" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>42</v>
       </c>
       <c r="B47" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="C47">
         <v>159974</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C48">
         <v>159963</v>
       </c>
       <c r="D48" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>44</v>
       </c>
       <c r="B49" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="C49">
         <v>159960</v>
       </c>
       <c r="D49" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E49" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>45</v>
       </c>
       <c r="B50" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="C50">
         <v>159971</v>
       </c>
       <c r="D50" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>46</v>
       </c>
       <c r="B51" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="C51">
         <v>159969</v>
       </c>
       <c r="D51" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E51" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>47</v>
       </c>
       <c r="B52" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="C52">
         <v>159963</v>
       </c>
       <c r="D52" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E52" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>48</v>
       </c>
       <c r="B53" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C53">
         <v>159968</v>
       </c>
       <c r="D53" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E53" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>49</v>
       </c>
       <c r="B54" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="C54">
         <v>159968</v>
       </c>
       <c r="D54" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>50</v>
       </c>
       <c r="B55" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C55">
         <v>160000</v>
       </c>
       <c r="D55" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="E55" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2647,419 +2633,419 @@
       <selection activeCell="A26" sqref="A26:A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="B2">
         <v>159975</v>
       </c>
     </row>
-    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>159976</v>
       </c>
     </row>
-    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>159963</v>
       </c>
     </row>
-    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>159964</v>
       </c>
     </row>
-    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>159975</v>
       </c>
     </row>
-    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>159964</v>
       </c>
     </row>
-    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>159975</v>
       </c>
     </row>
-    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>159974</v>
       </c>
     </row>
-    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>159980</v>
       </c>
     </row>
-    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>159971</v>
       </c>
     </row>
-    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>159958</v>
       </c>
     </row>
-    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>159971</v>
       </c>
     </row>
-    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>159965</v>
       </c>
     </row>
-    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>159970</v>
       </c>
     </row>
-    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>60</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>159967</v>
       </c>
     </row>
-    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>159966</v>
       </c>
     </row>
-    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>159975</v>
       </c>
     </row>
-    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>159974</v>
       </c>
     </row>
-    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>159961</v>
       </c>
     </row>
-    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>159966</v>
       </c>
     </row>
-    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>159963</v>
       </c>
     </row>
-    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>159972</v>
       </c>
     </row>
-    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>68</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>159974</v>
       </c>
     </row>
-    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>159954</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B26">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>71</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>159979</v>
       </c>
     </row>
-    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>159965</v>
       </c>
     </row>
-    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>159971</v>
       </c>
     </row>
-    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>74</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>159966</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B31">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>6</v>
       </c>
     </row>
-    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="B33">
         <v>159962</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B34">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="B35">
         <v>159960</v>
       </c>
     </row>
-    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="B36">
         <v>159960</v>
       </c>
     </row>
-    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>79</v>
+        <v>67</v>
       </c>
       <c r="B37">
         <v>159971</v>
       </c>
     </row>
-    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="B38">
         <v>159974</v>
       </c>
     </row>
-    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>69</v>
       </c>
       <c r="B39">
         <v>129199</v>
       </c>
     </row>
-    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B40">
         <v>159970</v>
       </c>
     </row>
-    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B41">
         <v>159978</v>
       </c>
     </row>
-    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="B42">
         <v>159965</v>
       </c>
     </row>
-    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B43">
         <v>159961</v>
       </c>
     </row>
-    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>85</v>
+        <v>73</v>
       </c>
       <c r="B44">
         <v>159975</v>
       </c>
     </row>
-    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="B45">
         <v>159964</v>
       </c>
     </row>
-    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="B46">
         <v>159961</v>
       </c>
     </row>
-    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B47">
         <v>159972</v>
       </c>
     </row>
-    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="B48">
         <v>159970</v>
       </c>
     </row>
-    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="B49">
         <v>159964</v>
       </c>
     </row>
-    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B50">
         <v>159969</v>
       </c>
     </row>
-    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="B51">
         <v>159969</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="B52">
         <v>2</v>

</xml_diff>